<commit_message>
Added import/export template for Kinerja
</commit_message>
<xml_diff>
--- a/storage/app/templates/kompetensi_template.xlsx
+++ b/storage/app/templates/kompetensi_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pmo-project\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16490B6-E5CE-48E4-A2C0-DA2A025C830F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3613CF7-85BD-423E-BB52-D600A194D1D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="5250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,24 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>NIP</t>
-  </si>
-  <si>
-    <t>Nama Lengkap</t>
-  </si>
-  <si>
-    <t>Unit Kerja</t>
-  </si>
-  <si>
-    <t>Jabatan</t>
-  </si>
-  <si>
-    <t>Pendidikan</t>
-  </si>
-  <si>
-    <t>Tanggal Lahir</t>
   </si>
   <si>
     <t>Tujuan Pemeriksaan</t>
@@ -148,6 +133,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -186,13 +172,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -533,205 +519,175 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-    </row>
-    <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="13">
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AB1"/>
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="X1:AA1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>